<commit_message>
Negative Login Test with ApachePOI completed
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/TestData.xlsx
+++ b/src/test/java/apachePOI/TestData.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\Intership-Project-Mersy.io\src\test\java\apachePOI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5FD313-4BD6-416B-8131-79891AD801C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="NegativeLoginTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,34 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+  <si>
+    <t>Student-5</t>
+  </si>
+  <si>
+    <t>S1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>S12345</t>
+  </si>
+  <si>
+    <t>Student_12345</t>
+  </si>
+  <si>
+    <t>Student_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +362,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
US011Steps payment data come from ExcelFile completed
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/TestData.xlsx
+++ b/src/test/java/apachePOI/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\Intership-Project-Mersy.io\src\test\java\apachePOI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5FD313-4BD6-416B-8131-79891AD801C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25392A0-C9D6-4E95-875B-7A3838B67EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NegativeLoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="CampusBankData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Student-5</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>4242 4242 4242 4242</t>
   </si>
 </sst>
 </file>
@@ -365,7 +369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -426,4 +430,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0385039A-AB0F-449D-84A7-12D92E84510F}">
+  <dimension ref="E10:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ParallelTestRunner SmokeTestRunner RegressionTestRunner AllTestRunner xmlTestRunner added
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/TestData.xlsx
+++ b/src/test/java/apachePOI/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\Intership-Project-Mersy.io\src\test\java\apachePOI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25392A0-C9D6-4E95-875B-7A3838B67EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DC71E8-025B-4D3E-8B59-16EE09DE2B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="0" windowWidth="23256" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NegativeLoginTest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Student-5</t>
   </si>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,17 +413,9 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -436,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0385039A-AB0F-449D-84A7-12D92E84510F}">
   <dimension ref="E10:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
US001.feature Locator Problem fixed
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/TestData.xlsx
+++ b/src/test/java/apachePOI/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\Intership-Project-Mersy.io\src\test\java\apachePOI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\Internship-Project-Mersy.io\src\test\java\apachePOI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DC71E8-025B-4D3E-8B59-16EE09DE2B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3691F34E-A897-4BF5-9F73-4BA45916479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="0" windowWidth="23256" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NegativeLoginTest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>Student-5</t>
   </si>
@@ -34,19 +34,7 @@
     <t>S1234</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>S12345</t>
-  </si>
-  <si>
-    <t>Student_12345</t>
-  </si>
-  <si>
     <t>Student_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>4242 4242 4242 4242</t>
@@ -389,34 +377,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -439,7 +427,7 @@
   <sheetData>
     <row r="10" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="5:7" x14ac:dyDescent="0.25">

</xml_diff>